<commit_message>
set meal update, selectable but not displayable yet
</commit_message>
<xml_diff>
--- a/menu_list.xlsx
+++ b/menu_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\2023S2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/lo0001ui_e_ntu_edu_sg/Documents/Y2/S2/SC2002 OOP/SC2002-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F5C744-94CF-4EEA-9F38-C8142AC726FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{26F5C744-94CF-4EEA-9F38-C8142AC726FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D439759-138A-424F-A03A-FED218EAB10C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
   <sheets>
     <sheet name="staff" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t>drink</t>
+  </si>
+  <si>
+    <t>Sphagetti</t>
+  </si>
+  <si>
+    <t>pasta</t>
+  </si>
+  <si>
+    <t>cheeseburger</t>
   </si>
 </sst>
 </file>
@@ -498,17 +507,17 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="A10:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -522,7 +531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -536,7 +545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -550,7 +559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -564,7 +573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -578,7 +587,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -592,7 +601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -606,7 +615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -620,7 +629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -634,232 +643,254 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>1.5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
     </row>
   </sheetData>

</xml_diff>